<commit_message>
Borders for most of the tables, moved to Routes - coCalculationRoutes.js
</commit_message>
<xml_diff>
--- a/backend/output.xlsx
+++ b/backend/output.xlsx
@@ -888,7 +888,7 @@
         <v>3</v>
       </c>
       <c r="I22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J22">
         <v>3</v>
@@ -941,7 +941,7 @@
         <v>100</v>
       </c>
       <c r="I23">
-        <v>66.67</v>
+        <v>100</v>
       </c>
       <c r="J23">
         <v>100</v>
@@ -1126,13 +1126,13 @@
         <v>CO2</v>
       </c>
       <c r="B29">
-        <v>83.34</v>
+        <v>91.67</v>
       </c>
       <c r="C29">
         <v>100</v>
       </c>
       <c r="D29">
-        <v>91.67</v>
+        <v>95.84</v>
       </c>
       <c r="E29">
         <v>3</v>
@@ -1159,7 +1159,7 @@
         <v>66.67</v>
       </c>
       <c r="O29">
-        <v>66.67</v>
+        <v>100</v>
       </c>
       <c r="P29" t="str">
         <v xml:space="preserve"> </v>
@@ -1168,7 +1168,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="R29">
-        <v>83.34</v>
+        <v>91.67</v>
       </c>
     </row>
     <row r="30">

</xml_diff>

<commit_message>
stashed xlsx, used exceljs to build excel file
</commit_message>
<xml_diff>
--- a/backend/output.xlsx
+++ b/backend/output.xlsx
@@ -2255,17 +2255,44 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B36:H36"/>
-    <mergeCell ref="I36:O36"/>
-    <mergeCell ref="B37:H37"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="I37:O37"/>
-    <mergeCell ref="I38:O38"/>
-    <mergeCell ref="I39:O39"/>
-    <mergeCell ref="M42:O42"/>
-    <mergeCell ref="J52:L52"/>
+  <mergeCells count="37">
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="D12:S12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="L8:P8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="L6:P6"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L5:P5"/>
+    <mergeCell ref="Q5:S5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>